<commit_message>
Starting out minor details for prediction date of week by month
</commit_message>
<xml_diff>
--- a/App Data - Prediction.xlsx
+++ b/App Data - Prediction.xlsx
@@ -9,14 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="Day of Week Prediction" sheetId="1" r:id="rId1"/>
-    <sheet name="Month Prediction" sheetId="2" r:id="rId2"/>
+    <sheet name="Month Prediction" sheetId="2" r:id="rId1"/>
+    <sheet name="Day of Week Prediction - March" sheetId="1" r:id="rId2"/>
+    <sheet name="Day of Week Pred Apr" sheetId="3" r:id="rId3"/>
+    <sheet name="Day of Week Pred may" sheetId="4" r:id="rId4"/>
+    <sheet name="Day of Week Pred June" sheetId="5" r:id="rId5"/>
+    <sheet name="Day of Week Pred July" sheetId="6" r:id="rId6"/>
+    <sheet name="Day of Week Pred Aug" sheetId="7" r:id="rId7"/>
+    <sheet name="Day of Week Pred Sept" sheetId="8" r:id="rId8"/>
+    <sheet name="Day of Week Pred Oct" sheetId="9" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="26">
   <si>
     <t>The question that will be asked here is if we can predict the next days app transaction based on today's app transactions.</t>
   </si>
@@ -103,12 +110,6 @@
   </si>
   <si>
     <t>Prediction for November using formula y = 0.2336x + 172.42</t>
-  </si>
-  <si>
-    <t>Value of r^2 is so low it doesn't look</t>
-  </si>
-  <si>
-    <t>like you can predict the value.</t>
   </si>
   <si>
     <t xml:space="preserve">Prediction of Money made for August using y = 0.2146x + 160.86 </t>
@@ -201,369 +202,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Day of Week Prediction'!$B$3:$H$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>394</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>364</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>403</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>408</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>352</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>352</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>401</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Day of Week Prediction'!$B$4:$H$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>364</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>403</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>408</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>352</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>352</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>401</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>394</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="377586096"/>
-        <c:axId val="377584976"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="377586096"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="377584976"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="377584976"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="377586096"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -783,11 +421,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="184756176"/>
-        <c:axId val="318398048"/>
+        <c:axId val="292211328"/>
+        <c:axId val="292211888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="184756176"/>
+        <c:axId val="292211328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -905,12 +543,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318398048"/>
+        <c:crossAx val="292211888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="318398048"/>
+        <c:axId val="292211888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1028,7 +666,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184756176"/>
+        <c:crossAx val="292211328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1077,7 +715,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1116,7 +754,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Month vs Next Months Transactions</a:t>
+              <a:t> Month vs Next Months Purchase Amount</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1279,11 +917,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="389078848"/>
-        <c:axId val="376766688"/>
+        <c:axId val="292214128"/>
+        <c:axId val="292214688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="389078848"/>
+        <c:axId val="292214128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1400,12 +1038,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376766688"/>
+        <c:crossAx val="292214688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="376766688"/>
+        <c:axId val="292214688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1523,7 +1161,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="389078848"/>
+        <c:crossAx val="292214128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1613,46 +1251,6 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2724,558 +2322,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>319087</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>471487</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3495,6 +2542,1106 @@
             <v>1.04</v>
           </cell>
         </row>
+        <row r="9">
+          <cell r="A9">
+            <v>41488</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>41488</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>41488</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>41488</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>41488</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>41489</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>41489</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>41489</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>41489</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>41489</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>41489</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>41489</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>41489</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>41489</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>41489</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>41490</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>41490</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>41490</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>41490</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>41490</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>41490</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>41490</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>41490</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32">
+            <v>41491</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33">
+            <v>41491</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34">
+            <v>41491</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35">
+            <v>41491</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36">
+            <v>41492</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37">
+            <v>41492</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38">
+            <v>41492</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39">
+            <v>41492</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40">
+            <v>41492</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41">
+            <v>41492</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42">
+            <v>41492</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43">
+            <v>41492</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44">
+            <v>41492</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45">
+            <v>41492</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46">
+            <v>41493</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47">
+            <v>41493</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48">
+            <v>41493</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49">
+            <v>41493</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50">
+            <v>41493</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51">
+            <v>41493</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52">
+            <v>41493</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53">
+            <v>41493</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54">
+            <v>41494</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55">
+            <v>41494</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56">
+            <v>41494</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57">
+            <v>41494</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58">
+            <v>41494</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59">
+            <v>41494</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60">
+            <v>41494</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61">
+            <v>41494</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62">
+            <v>41494</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63">
+            <v>41495</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64">
+            <v>41495</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65">
+            <v>41495</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66">
+            <v>41495</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67">
+            <v>41495</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68">
+            <v>41495</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69">
+            <v>41495</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70">
+            <v>41496</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="A71">
+            <v>41496</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="A72">
+            <v>41496</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73">
+            <v>41496</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74">
+            <v>41496</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75">
+            <v>41496</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76">
+            <v>41496</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77">
+            <v>41497</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78">
+            <v>41497</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79">
+            <v>41497</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80">
+            <v>41497</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81">
+            <v>41497</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82">
+            <v>41497</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83">
+            <v>41497</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84">
+            <v>41497</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85">
+            <v>41498</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="A86">
+            <v>41498</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="A87">
+            <v>41498</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="A88">
+            <v>41498</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="A89">
+            <v>41498</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="A90">
+            <v>41498</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="A91">
+            <v>41498</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="A92">
+            <v>41499</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="A93">
+            <v>41499</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="A94">
+            <v>41499</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="A95">
+            <v>41499</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="A96">
+            <v>41499</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="A97">
+            <v>41499</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="A98">
+            <v>41499</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="A99">
+            <v>41499</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="A100">
+            <v>41499</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="A101">
+            <v>41499</v>
+          </cell>
+        </row>
+        <row r="102">
+          <cell r="A102">
+            <v>41499</v>
+          </cell>
+        </row>
+        <row r="103">
+          <cell r="A103">
+            <v>41499</v>
+          </cell>
+        </row>
+        <row r="104">
+          <cell r="A104">
+            <v>41499</v>
+          </cell>
+        </row>
+        <row r="105">
+          <cell r="A105">
+            <v>41499</v>
+          </cell>
+        </row>
+        <row r="106">
+          <cell r="A106">
+            <v>41500</v>
+          </cell>
+        </row>
+        <row r="107">
+          <cell r="A107">
+            <v>41500</v>
+          </cell>
+        </row>
+        <row r="108">
+          <cell r="A108">
+            <v>41500</v>
+          </cell>
+        </row>
+        <row r="109">
+          <cell r="A109">
+            <v>41500</v>
+          </cell>
+        </row>
+        <row r="110">
+          <cell r="A110">
+            <v>41500</v>
+          </cell>
+        </row>
+        <row r="111">
+          <cell r="A111">
+            <v>41500</v>
+          </cell>
+        </row>
+        <row r="112">
+          <cell r="A112">
+            <v>41501</v>
+          </cell>
+        </row>
+        <row r="113">
+          <cell r="A113">
+            <v>41501</v>
+          </cell>
+        </row>
+        <row r="114">
+          <cell r="A114">
+            <v>41501</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="A115">
+            <v>41501</v>
+          </cell>
+        </row>
+        <row r="116">
+          <cell r="A116">
+            <v>41501</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="A117">
+            <v>41501</v>
+          </cell>
+        </row>
+        <row r="118">
+          <cell r="A118">
+            <v>41502</v>
+          </cell>
+        </row>
+        <row r="119">
+          <cell r="A119">
+            <v>41502</v>
+          </cell>
+        </row>
+        <row r="120">
+          <cell r="A120">
+            <v>41502</v>
+          </cell>
+        </row>
+        <row r="121">
+          <cell r="A121">
+            <v>41502</v>
+          </cell>
+        </row>
+        <row r="122">
+          <cell r="A122">
+            <v>41502</v>
+          </cell>
+        </row>
+        <row r="123">
+          <cell r="A123">
+            <v>41502</v>
+          </cell>
+        </row>
+        <row r="124">
+          <cell r="A124">
+            <v>41502</v>
+          </cell>
+        </row>
+        <row r="125">
+          <cell r="A125">
+            <v>41503</v>
+          </cell>
+        </row>
+        <row r="126">
+          <cell r="A126">
+            <v>41503</v>
+          </cell>
+        </row>
+        <row r="127">
+          <cell r="A127">
+            <v>41503</v>
+          </cell>
+        </row>
+        <row r="128">
+          <cell r="A128">
+            <v>41503</v>
+          </cell>
+        </row>
+        <row r="129">
+          <cell r="A129">
+            <v>41503</v>
+          </cell>
+        </row>
+        <row r="130">
+          <cell r="A130">
+            <v>41503</v>
+          </cell>
+        </row>
+        <row r="131">
+          <cell r="A131">
+            <v>41503</v>
+          </cell>
+        </row>
+        <row r="132">
+          <cell r="A132">
+            <v>41504</v>
+          </cell>
+        </row>
+        <row r="133">
+          <cell r="A133">
+            <v>41504</v>
+          </cell>
+        </row>
+        <row r="134">
+          <cell r="A134">
+            <v>41504</v>
+          </cell>
+        </row>
+        <row r="135">
+          <cell r="A135">
+            <v>41504</v>
+          </cell>
+        </row>
+        <row r="136">
+          <cell r="A136">
+            <v>41504</v>
+          </cell>
+        </row>
+        <row r="137">
+          <cell r="A137">
+            <v>41504</v>
+          </cell>
+        </row>
+        <row r="138">
+          <cell r="A138">
+            <v>41504</v>
+          </cell>
+        </row>
+        <row r="139">
+          <cell r="A139">
+            <v>41504</v>
+          </cell>
+        </row>
+        <row r="140">
+          <cell r="A140">
+            <v>41504</v>
+          </cell>
+        </row>
+        <row r="141">
+          <cell r="A141">
+            <v>41505</v>
+          </cell>
+        </row>
+        <row r="142">
+          <cell r="A142">
+            <v>41505</v>
+          </cell>
+        </row>
+        <row r="143">
+          <cell r="A143">
+            <v>41505</v>
+          </cell>
+        </row>
+        <row r="144">
+          <cell r="A144">
+            <v>41505</v>
+          </cell>
+        </row>
+        <row r="145">
+          <cell r="A145">
+            <v>41505</v>
+          </cell>
+        </row>
+        <row r="146">
+          <cell r="A146">
+            <v>41505</v>
+          </cell>
+        </row>
+        <row r="147">
+          <cell r="A147">
+            <v>41505</v>
+          </cell>
+        </row>
+        <row r="148">
+          <cell r="A148">
+            <v>41505</v>
+          </cell>
+        </row>
+        <row r="149">
+          <cell r="A149">
+            <v>41506</v>
+          </cell>
+        </row>
+        <row r="150">
+          <cell r="A150">
+            <v>41506</v>
+          </cell>
+        </row>
+        <row r="151">
+          <cell r="A151">
+            <v>41506</v>
+          </cell>
+        </row>
+        <row r="152">
+          <cell r="A152">
+            <v>41506</v>
+          </cell>
+        </row>
+        <row r="153">
+          <cell r="A153">
+            <v>41506</v>
+          </cell>
+        </row>
+        <row r="154">
+          <cell r="A154">
+            <v>41506</v>
+          </cell>
+        </row>
+        <row r="155">
+          <cell r="A155">
+            <v>41506</v>
+          </cell>
+        </row>
+        <row r="156">
+          <cell r="A156">
+            <v>41506</v>
+          </cell>
+        </row>
+        <row r="157">
+          <cell r="A157">
+            <v>41506</v>
+          </cell>
+        </row>
+        <row r="158">
+          <cell r="A158">
+            <v>41506</v>
+          </cell>
+        </row>
+        <row r="159">
+          <cell r="A159">
+            <v>41506</v>
+          </cell>
+        </row>
+        <row r="160">
+          <cell r="A160">
+            <v>41506</v>
+          </cell>
+        </row>
+        <row r="161">
+          <cell r="A161">
+            <v>41506</v>
+          </cell>
+        </row>
+        <row r="162">
+          <cell r="A162">
+            <v>41507</v>
+          </cell>
+        </row>
+        <row r="163">
+          <cell r="A163">
+            <v>41507</v>
+          </cell>
+        </row>
+        <row r="164">
+          <cell r="A164">
+            <v>41507</v>
+          </cell>
+        </row>
+        <row r="165">
+          <cell r="A165">
+            <v>41507</v>
+          </cell>
+        </row>
+        <row r="166">
+          <cell r="A166">
+            <v>41507</v>
+          </cell>
+        </row>
+        <row r="167">
+          <cell r="A167">
+            <v>41508</v>
+          </cell>
+        </row>
+        <row r="168">
+          <cell r="A168">
+            <v>41508</v>
+          </cell>
+        </row>
+        <row r="169">
+          <cell r="A169">
+            <v>41508</v>
+          </cell>
+        </row>
+        <row r="170">
+          <cell r="A170">
+            <v>41508</v>
+          </cell>
+        </row>
+        <row r="171">
+          <cell r="A171">
+            <v>41509</v>
+          </cell>
+        </row>
+        <row r="172">
+          <cell r="A172">
+            <v>41509</v>
+          </cell>
+        </row>
+        <row r="173">
+          <cell r="A173">
+            <v>41509</v>
+          </cell>
+        </row>
+        <row r="174">
+          <cell r="A174">
+            <v>41510</v>
+          </cell>
+        </row>
+        <row r="175">
+          <cell r="A175">
+            <v>41510</v>
+          </cell>
+        </row>
+        <row r="176">
+          <cell r="A176">
+            <v>41510</v>
+          </cell>
+        </row>
+        <row r="177">
+          <cell r="A177">
+            <v>41510</v>
+          </cell>
+        </row>
+        <row r="178">
+          <cell r="A178">
+            <v>41510</v>
+          </cell>
+        </row>
+        <row r="179">
+          <cell r="A179">
+            <v>41510</v>
+          </cell>
+        </row>
+        <row r="180">
+          <cell r="A180">
+            <v>41511</v>
+          </cell>
+        </row>
+        <row r="181">
+          <cell r="A181">
+            <v>41511</v>
+          </cell>
+        </row>
+        <row r="182">
+          <cell r="A182">
+            <v>41511</v>
+          </cell>
+        </row>
+        <row r="183">
+          <cell r="A183">
+            <v>41511</v>
+          </cell>
+        </row>
+        <row r="184">
+          <cell r="A184">
+            <v>41511</v>
+          </cell>
+        </row>
+        <row r="185">
+          <cell r="A185">
+            <v>41511</v>
+          </cell>
+        </row>
+        <row r="186">
+          <cell r="A186">
+            <v>41511</v>
+          </cell>
+        </row>
+        <row r="187">
+          <cell r="A187">
+            <v>41511</v>
+          </cell>
+        </row>
+        <row r="188">
+          <cell r="A188">
+            <v>41512</v>
+          </cell>
+        </row>
+        <row r="189">
+          <cell r="A189">
+            <v>41512</v>
+          </cell>
+        </row>
+        <row r="190">
+          <cell r="A190">
+            <v>41512</v>
+          </cell>
+        </row>
+        <row r="191">
+          <cell r="A191">
+            <v>41512</v>
+          </cell>
+        </row>
+        <row r="192">
+          <cell r="A192">
+            <v>41512</v>
+          </cell>
+        </row>
+        <row r="193">
+          <cell r="A193">
+            <v>41512</v>
+          </cell>
+        </row>
+        <row r="194">
+          <cell r="A194">
+            <v>41512</v>
+          </cell>
+        </row>
+        <row r="195">
+          <cell r="A195">
+            <v>41512</v>
+          </cell>
+        </row>
+        <row r="196">
+          <cell r="A196">
+            <v>41513</v>
+          </cell>
+        </row>
+        <row r="197">
+          <cell r="A197">
+            <v>41513</v>
+          </cell>
+        </row>
+        <row r="198">
+          <cell r="A198">
+            <v>41513</v>
+          </cell>
+        </row>
+        <row r="199">
+          <cell r="A199">
+            <v>41513</v>
+          </cell>
+        </row>
+        <row r="200">
+          <cell r="A200">
+            <v>41513</v>
+          </cell>
+        </row>
+        <row r="201">
+          <cell r="A201">
+            <v>41513</v>
+          </cell>
+        </row>
+        <row r="202">
+          <cell r="A202">
+            <v>41513</v>
+          </cell>
+        </row>
+        <row r="203">
+          <cell r="A203">
+            <v>41513</v>
+          </cell>
+        </row>
+        <row r="204">
+          <cell r="A204">
+            <v>41513</v>
+          </cell>
+        </row>
+        <row r="205">
+          <cell r="A205">
+            <v>41514</v>
+          </cell>
+        </row>
+        <row r="206">
+          <cell r="A206">
+            <v>41514</v>
+          </cell>
+        </row>
+        <row r="207">
+          <cell r="A207">
+            <v>41514</v>
+          </cell>
+        </row>
+        <row r="208">
+          <cell r="A208">
+            <v>41514</v>
+          </cell>
+        </row>
+        <row r="209">
+          <cell r="A209">
+            <v>41514</v>
+          </cell>
+        </row>
+        <row r="210">
+          <cell r="A210">
+            <v>41514</v>
+          </cell>
+        </row>
+        <row r="211">
+          <cell r="A211">
+            <v>41514</v>
+          </cell>
+        </row>
+        <row r="212">
+          <cell r="A212">
+            <v>41514</v>
+          </cell>
+        </row>
+        <row r="213">
+          <cell r="A213">
+            <v>41514</v>
+          </cell>
+        </row>
+        <row r="214">
+          <cell r="A214">
+            <v>41514</v>
+          </cell>
+        </row>
+        <row r="216">
+          <cell r="A216">
+            <v>41515</v>
+          </cell>
+        </row>
+        <row r="217">
+          <cell r="A217">
+            <v>41515</v>
+          </cell>
+        </row>
+        <row r="218">
+          <cell r="A218">
+            <v>41515</v>
+          </cell>
+        </row>
+        <row r="219">
+          <cell r="A219">
+            <v>41515</v>
+          </cell>
+        </row>
+        <row r="220">
+          <cell r="A220">
+            <v>41515</v>
+          </cell>
+        </row>
+        <row r="221">
+          <cell r="A221">
+            <v>41515</v>
+          </cell>
+        </row>
+        <row r="222">
+          <cell r="A222">
+            <v>41516</v>
+          </cell>
+        </row>
+        <row r="223">
+          <cell r="A223">
+            <v>41516</v>
+          </cell>
+        </row>
+        <row r="224">
+          <cell r="A224">
+            <v>41516</v>
+          </cell>
+        </row>
+        <row r="225">
+          <cell r="A225">
+            <v>41516</v>
+          </cell>
+        </row>
+        <row r="226">
+          <cell r="A226">
+            <v>41517</v>
+          </cell>
+        </row>
+        <row r="227">
+          <cell r="A227">
+            <v>41517</v>
+          </cell>
+        </row>
+        <row r="228">
+          <cell r="A228">
+            <v>41517</v>
+          </cell>
+        </row>
+        <row r="229">
+          <cell r="A229">
+            <v>41517</v>
+          </cell>
+        </row>
         <row r="230">
           <cell r="A230">
             <v>41517</v>
@@ -3528,90 +3675,13 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="10">
-        <row r="2">
-          <cell r="A2">
-            <v>41343</v>
-          </cell>
-        </row>
-        <row r="395">
-          <cell r="A395">
-            <v>41574</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="11">
-        <row r="2">
-          <cell r="A2">
-            <v>41344</v>
-          </cell>
-        </row>
-        <row r="365">
-          <cell r="A365">
-            <v>41575</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="12">
-        <row r="2">
-          <cell r="A2">
-            <v>41338</v>
-          </cell>
-        </row>
-        <row r="404">
-          <cell r="A404">
-            <v>41576</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="13">
-        <row r="2">
-          <cell r="A2">
-            <v>41339</v>
-          </cell>
-        </row>
-        <row r="409">
-          <cell r="A409">
-            <v>41577</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="14">
-        <row r="2">
-          <cell r="A2">
-            <v>41340</v>
-          </cell>
-        </row>
-        <row r="353">
-          <cell r="A353">
-            <v>41578</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="15">
-        <row r="2">
-          <cell r="A2">
-            <v>41341</v>
-          </cell>
-        </row>
-        <row r="353">
-          <cell r="A353">
-            <v>41572</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="16">
-        <row r="2">
-          <cell r="A2">
-            <v>41335</v>
-          </cell>
-        </row>
-        <row r="402">
-          <cell r="A402">
-            <v>41573</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
       <sheetData sheetId="19"/>
@@ -3911,133 +3981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1">
-        <f>COUNT([1]Sunday!$A$2:'[1]Sunday'!$A$395)</f>
-        <v>394</v>
-      </c>
-      <c r="C3" s="1">
-        <f>COUNT([1]Monday!$A$2:'[1]Monday'!$A$365)</f>
-        <v>364</v>
-      </c>
-      <c r="D3" s="1">
-        <f>COUNT([1]Tuesday!$A$2:'[1]Tuesday'!$A$404)</f>
-        <v>403</v>
-      </c>
-      <c r="E3" s="1">
-        <f>COUNT([1]Wednesday!$A$2:'[1]Wednesday'!$A$409)</f>
-        <v>408</v>
-      </c>
-      <c r="F3" s="1">
-        <f>COUNT([1]Thursday!$A$2:'[1]Thursday'!$A$353)</f>
-        <v>352</v>
-      </c>
-      <c r="G3" s="1">
-        <f>COUNT([1]Friday!$A$2:'[1]Friday'!$A$353)</f>
-        <v>352</v>
-      </c>
-      <c r="H3" s="1">
-        <f>COUNT([1]Saturday!$A$2:'[1]Saturday'!$A$402)</f>
-        <v>401</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="1">
-        <f>COUNT([1]Monday!$A$2:'[1]Monday'!$A$365)</f>
-        <v>364</v>
-      </c>
-      <c r="C4" s="1">
-        <f>COUNT([1]Tuesday!$A$2:'[1]Tuesday'!$A$404)</f>
-        <v>403</v>
-      </c>
-      <c r="D4" s="1">
-        <f>COUNT([1]Wednesday!$A$2:'[1]Wednesday'!$A$409)</f>
-        <v>408</v>
-      </c>
-      <c r="E4" s="1">
-        <f>COUNT([1]Thursday!$A$2:'[1]Thursday'!$A$353)</f>
-        <v>352</v>
-      </c>
-      <c r="F4" s="1">
-        <f>COUNT([1]Friday!$A$2:'[1]Friday'!$A$353)</f>
-        <v>352</v>
-      </c>
-      <c r="G4" s="1">
-        <f>COUNT([1]Saturday!$A$2:'[1]Saturday'!$A$402)</f>
-        <v>401</v>
-      </c>
-      <c r="H4" s="1">
-        <f>COUNT([1]Sunday!$A$2:'[1]Sunday'!$A$395)</f>
-        <v>394</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4083,7 +4030,7 @@
       </c>
       <c r="B3" s="3">
         <f>COUNT([1]March!$A$2:'[1]March'!$A$795)</f>
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C3" s="1">
         <f>COUNT([1]April!$A$2:'[1]April'!$A$462)</f>
@@ -4214,7 +4161,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -4243,4 +4190,2129 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="F16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="G17">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="H18">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="E22">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="F23">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="G24">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="H25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="D28">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="E29">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="F30">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="G31">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="H32">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="G14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="F20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="G21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="H22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="D25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="F27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="G28">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="H29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="G12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="G19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="H20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="E24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="F25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="H27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="D30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="E31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="F32">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="G23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="F29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="G30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="H31">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="G14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="F20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="G21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="H22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="D25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="E26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="G28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="H29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="D32">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <f>COUNT([1]August!$A$9:$A$13)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <f>COUNT([1]August!$A$14:$A$23)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <f>COUNT([1]August!$A$24:$A$31)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f>COUNT([1]August!$A$32:$A$35)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f>COUNT([1]August!$A$36:$A$45)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <f>COUNT([1]August!$A$46:$A$53)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <f>COUNT([1]August!$A$54:$A$62)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <f>COUNT([1]August!$A$63:$A$69)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <f>COUNT([1]August!$A$70:$A$76)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="H12">
+        <f>COUNT([1]August!$A$77:$A$84)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f>COUNT([1]August!$A$85:$A$91)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <f>COUNT([1]August!$A$92:$A$105)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <f>COUNT([1]August!$A$106:$A$111)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <f>COUNT([1]August!$A$112:$A$117)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <f>COUNT([1]August!$A$118:$A$124)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="G18">
+        <f>COUNT([1]August!$A$125:$A$131)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="H19">
+        <f>COUNT([1]August!$A$132:$A$140)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <f>COUNT([1]August!$A$141:$A$148)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <f>COUNT([1]August!$A$149:$A$161)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <f>COUNT([1]August!$A$162:$A$166)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="E23">
+        <f>COUNT([1]August!$A$167:$A$170)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="F24">
+        <f>COUNT([1]August!$A$171:$A$173)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="G25">
+        <f>COUNT([1]August!$A$174:$A$179)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="H26">
+        <f>COUNT([1]August!$A$180:$A$187)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <f>COUNT([1]August!$A$188:$A$195)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <f>COUNT([1]August!$A$196:$A$204)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="D29">
+        <f>COUNT([1]August!$A$205:$A$214)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="E30">
+        <f>COUNT([1]August!$A$216:$A$221)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="F31">
+        <f>COUNT([1]August!$A$222:$A$225)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="G32">
+        <f>COUNT([1]August!$A$226:$A$230)</f>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
one more month down
</commit_message>
<xml_diff>
--- a/App Data - Prediction.xlsx
+++ b/App Data - Prediction.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Month Prediction" sheetId="2" r:id="rId1"/>
@@ -421,11 +421,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="292211328"/>
-        <c:axId val="292211888"/>
+        <c:axId val="253326752"/>
+        <c:axId val="253331792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="292211328"/>
+        <c:axId val="253326752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -543,12 +543,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292211888"/>
+        <c:crossAx val="253331792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="292211888"/>
+        <c:axId val="253331792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -666,7 +666,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292211328"/>
+        <c:crossAx val="253326752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -917,11 +917,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="292214128"/>
-        <c:axId val="292214688"/>
+        <c:axId val="253329552"/>
+        <c:axId val="253328992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="292214128"/>
+        <c:axId val="253329552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1038,12 +1038,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292214688"/>
+        <c:crossAx val="253328992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="292214688"/>
+        <c:axId val="253328992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1161,7 +1161,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292214128"/>
+        <c:crossAx val="253329552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2441,8 +2441,8 @@
       <sheetName val="Day 31"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2">
         <row r="2">
           <cell r="A2">
@@ -3675,44 +3675,44 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4197,7 +4197,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5619,8 +5619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5933,10 +5933,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H32"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5968,155 +5968,240 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="G8">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
+      <c r="B31">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -6128,7 +6213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added more things to the report and necessary items which were pointed out by Prof Kamali
</commit_message>
<xml_diff>
--- a/App Data - Prediction.xlsx
+++ b/App Data - Prediction.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755"/>
   </bookViews>
   <sheets>
     <sheet name="Month Prediction" sheetId="2" r:id="rId1"/>
@@ -187,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -197,6 +197,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,11 +435,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="239502368"/>
-        <c:axId val="239505168"/>
+        <c:axId val="1333934224"/>
+        <c:axId val="1333932048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="239502368"/>
+        <c:axId val="1333934224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -556,12 +557,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239505168"/>
+        <c:crossAx val="1333932048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="239505168"/>
+        <c:axId val="1333932048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +680,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239502368"/>
+        <c:crossAx val="1333934224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -885,16 +886,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>426.87908600000213</c:v>
+                  <c:v>426.87</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>253.22090599999942</c:v>
+                  <c:v>253.22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>212.50666799999968</c:v>
+                  <c:v>212.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>202.74083299999978</c:v>
+                  <c:v>202.74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -906,16 +907,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>253.22090599999942</c:v>
+                  <c:v>253.22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>212.50666799999968</c:v>
+                  <c:v>212.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>202.74083299999978</c:v>
+                  <c:v>202.74</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>209.99964299999974</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -930,11 +931,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="240247872"/>
-        <c:axId val="240247312"/>
+        <c:axId val="1333934768"/>
+        <c:axId val="1333933136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="240247872"/>
+        <c:axId val="1333934768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1051,12 +1052,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240247312"/>
+        <c:crossAx val="1333933136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="240247312"/>
+        <c:axId val="1333933136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1174,7 +1175,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240247872"/>
+        <c:crossAx val="1333934768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1843,94 +1844,94 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="184">
                   <c:v>5</c:v>
@@ -2581,94 +2582,94 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="183">
                   <c:v>5</c:v>
@@ -2866,11 +2867,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="381140576"/>
-        <c:axId val="380271472"/>
+        <c:axId val="1333938576"/>
+        <c:axId val="1333939120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="381140576"/>
+        <c:axId val="1333938576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2891,6 +2892,31 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Todays Amount</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
@@ -2958,12 +2984,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="380271472"/>
+        <c:crossAx val="1333939120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="380271472"/>
+        <c:axId val="1333939120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2984,6 +3010,36 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tomorrow's</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Amount</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
@@ -3051,7 +3107,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381140576"/>
+        <c:crossAx val="1333938576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4872,1328 +4928,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Statistical Summary"/>
-      <sheetName val="AppData"/>
-      <sheetName val="March"/>
-      <sheetName val="April"/>
-      <sheetName val="May"/>
-      <sheetName val="June"/>
-      <sheetName val="July"/>
-      <sheetName val="August"/>
-      <sheetName val="September"/>
-      <sheetName val="October"/>
-      <sheetName val="Sunday"/>
-      <sheetName val="Monday"/>
-      <sheetName val="Tuesday"/>
-      <sheetName val="Wednesday"/>
-      <sheetName val="Thursday"/>
-      <sheetName val="Friday"/>
-      <sheetName val="Saturday"/>
-      <sheetName val="Day 1"/>
-      <sheetName val="Day 2"/>
-      <sheetName val="Day 3"/>
-      <sheetName val="Day 4"/>
-      <sheetName val="Day 5"/>
-      <sheetName val="Day 6"/>
-      <sheetName val="Day 7"/>
-      <sheetName val="Day 8"/>
-      <sheetName val="Day 9"/>
-      <sheetName val="Day 10"/>
-      <sheetName val="Day 11"/>
-      <sheetName val="Day 12"/>
-      <sheetName val="Day 13"/>
-      <sheetName val="Day 14"/>
-      <sheetName val="Day 15"/>
-      <sheetName val="Day 16"/>
-      <sheetName val="Day 17"/>
-      <sheetName val="Day 18"/>
-      <sheetName val="Day 19"/>
-      <sheetName val="Day 20"/>
-      <sheetName val="Day 21"/>
-      <sheetName val="Day 22"/>
-      <sheetName val="Day 23"/>
-      <sheetName val="Day 24"/>
-      <sheetName val="Day 25"/>
-      <sheetName val="Day 26"/>
-      <sheetName val="Day 27"/>
-      <sheetName val="Day 28"/>
-      <sheetName val="Day 29"/>
-      <sheetName val="Day 30"/>
-      <sheetName val="Day 31"/>
+      <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="A2">
-            <v>41335</v>
-          </cell>
-          <cell r="J2">
-            <v>1.04</v>
-          </cell>
-        </row>
-        <row r="795">
-          <cell r="A795">
-            <v>41364</v>
-          </cell>
-          <cell r="J795">
-            <v>1.04</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3">
-        <row r="2">
-          <cell r="A2">
-            <v>41365</v>
-          </cell>
-          <cell r="J2">
-            <v>1.04</v>
-          </cell>
-        </row>
-        <row r="462">
-          <cell r="A462">
-            <v>41394</v>
-          </cell>
-          <cell r="J462">
-            <v>1.000909</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4">
-        <row r="2">
-          <cell r="A2">
-            <v>41395</v>
-          </cell>
-          <cell r="J2">
-            <v>1.04</v>
-          </cell>
-        </row>
-        <row r="285">
-          <cell r="A285">
-            <v>41425</v>
-          </cell>
-          <cell r="J285">
-            <v>1.04</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5">
-        <row r="2">
-          <cell r="A2">
-            <v>41426</v>
-          </cell>
-          <cell r="J2">
-            <v>-1.04</v>
-          </cell>
-        </row>
-        <row r="229">
-          <cell r="A229">
-            <v>41455</v>
-          </cell>
-          <cell r="J229">
-            <v>1.04</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6">
-        <row r="2">
-          <cell r="A2">
-            <v>41456</v>
-          </cell>
-          <cell r="J2">
-            <v>1.04</v>
-          </cell>
-        </row>
-        <row r="239">
-          <cell r="A239">
-            <v>41486</v>
-          </cell>
-          <cell r="J239">
-            <v>1.04</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7">
-        <row r="2">
-          <cell r="A2">
-            <v>41487</v>
-          </cell>
-          <cell r="J2">
-            <v>1.04</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>41488</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>41488</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>41488</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>41488</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>41488</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>41489</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>41489</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>41489</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>41489</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>41489</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>41489</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>41489</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>41489</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>41489</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23">
-            <v>41489</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24">
-            <v>41490</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25">
-            <v>41490</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26">
-            <v>41490</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27">
-            <v>41490</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28">
-            <v>41490</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29">
-            <v>41490</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30">
-            <v>41490</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31">
-            <v>41490</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32">
-            <v>41491</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33">
-            <v>41491</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34">
-            <v>41491</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35">
-            <v>41491</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36">
-            <v>41492</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37">
-            <v>41492</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38">
-            <v>41492</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39">
-            <v>41492</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40">
-            <v>41492</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41">
-            <v>41492</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42">
-            <v>41492</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="A43">
-            <v>41492</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="A44">
-            <v>41492</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="A45">
-            <v>41492</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="A46">
-            <v>41493</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="A47">
-            <v>41493</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="A48">
-            <v>41493</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="A49">
-            <v>41493</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="A50">
-            <v>41493</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="A51">
-            <v>41493</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="A52">
-            <v>41493</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="A53">
-            <v>41493</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="A54">
-            <v>41494</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="A55">
-            <v>41494</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="A56">
-            <v>41494</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="A57">
-            <v>41494</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="A58">
-            <v>41494</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="A59">
-            <v>41494</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="A60">
-            <v>41494</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="A61">
-            <v>41494</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="A62">
-            <v>41494</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="A63">
-            <v>41495</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="A64">
-            <v>41495</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="A65">
-            <v>41495</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="A66">
-            <v>41495</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="A67">
-            <v>41495</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="A68">
-            <v>41495</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="A69">
-            <v>41495</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="A70">
-            <v>41496</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="A71">
-            <v>41496</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="A72">
-            <v>41496</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="A73">
-            <v>41496</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="A74">
-            <v>41496</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="A75">
-            <v>41496</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="A76">
-            <v>41496</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="A77">
-            <v>41497</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="A78">
-            <v>41497</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="A79">
-            <v>41497</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="A80">
-            <v>41497</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="A81">
-            <v>41497</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="A82">
-            <v>41497</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="A83">
-            <v>41497</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="A84">
-            <v>41497</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="A85">
-            <v>41498</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="A86">
-            <v>41498</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="A87">
-            <v>41498</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="A88">
-            <v>41498</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="A89">
-            <v>41498</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="A90">
-            <v>41498</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="A91">
-            <v>41498</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="A92">
-            <v>41499</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="A93">
-            <v>41499</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="A94">
-            <v>41499</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="A95">
-            <v>41499</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="A96">
-            <v>41499</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="A97">
-            <v>41499</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="A98">
-            <v>41499</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="A99">
-            <v>41499</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="A100">
-            <v>41499</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="A101">
-            <v>41499</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="A102">
-            <v>41499</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="A103">
-            <v>41499</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="A104">
-            <v>41499</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="A105">
-            <v>41499</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="A106">
-            <v>41500</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="A107">
-            <v>41500</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="A108">
-            <v>41500</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="A109">
-            <v>41500</v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="A110">
-            <v>41500</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="A111">
-            <v>41500</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="A112">
-            <v>41501</v>
-          </cell>
-        </row>
-        <row r="113">
-          <cell r="A113">
-            <v>41501</v>
-          </cell>
-        </row>
-        <row r="114">
-          <cell r="A114">
-            <v>41501</v>
-          </cell>
-        </row>
-        <row r="115">
-          <cell r="A115">
-            <v>41501</v>
-          </cell>
-        </row>
-        <row r="116">
-          <cell r="A116">
-            <v>41501</v>
-          </cell>
-        </row>
-        <row r="117">
-          <cell r="A117">
-            <v>41501</v>
-          </cell>
-        </row>
-        <row r="118">
-          <cell r="A118">
-            <v>41502</v>
-          </cell>
-        </row>
-        <row r="119">
-          <cell r="A119">
-            <v>41502</v>
-          </cell>
-        </row>
-        <row r="120">
-          <cell r="A120">
-            <v>41502</v>
-          </cell>
-        </row>
-        <row r="121">
-          <cell r="A121">
-            <v>41502</v>
-          </cell>
-        </row>
-        <row r="122">
-          <cell r="A122">
-            <v>41502</v>
-          </cell>
-        </row>
-        <row r="123">
-          <cell r="A123">
-            <v>41502</v>
-          </cell>
-        </row>
-        <row r="124">
-          <cell r="A124">
-            <v>41502</v>
-          </cell>
-        </row>
-        <row r="125">
-          <cell r="A125">
-            <v>41503</v>
-          </cell>
-        </row>
-        <row r="126">
-          <cell r="A126">
-            <v>41503</v>
-          </cell>
-        </row>
-        <row r="127">
-          <cell r="A127">
-            <v>41503</v>
-          </cell>
-        </row>
-        <row r="128">
-          <cell r="A128">
-            <v>41503</v>
-          </cell>
-        </row>
-        <row r="129">
-          <cell r="A129">
-            <v>41503</v>
-          </cell>
-        </row>
-        <row r="130">
-          <cell r="A130">
-            <v>41503</v>
-          </cell>
-        </row>
-        <row r="131">
-          <cell r="A131">
-            <v>41503</v>
-          </cell>
-        </row>
-        <row r="132">
-          <cell r="A132">
-            <v>41504</v>
-          </cell>
-        </row>
-        <row r="133">
-          <cell r="A133">
-            <v>41504</v>
-          </cell>
-        </row>
-        <row r="134">
-          <cell r="A134">
-            <v>41504</v>
-          </cell>
-        </row>
-        <row r="135">
-          <cell r="A135">
-            <v>41504</v>
-          </cell>
-        </row>
-        <row r="136">
-          <cell r="A136">
-            <v>41504</v>
-          </cell>
-        </row>
-        <row r="137">
-          <cell r="A137">
-            <v>41504</v>
-          </cell>
-        </row>
-        <row r="138">
-          <cell r="A138">
-            <v>41504</v>
-          </cell>
-        </row>
-        <row r="139">
-          <cell r="A139">
-            <v>41504</v>
-          </cell>
-        </row>
-        <row r="140">
-          <cell r="A140">
-            <v>41504</v>
-          </cell>
-        </row>
-        <row r="141">
-          <cell r="A141">
-            <v>41505</v>
-          </cell>
-        </row>
-        <row r="142">
-          <cell r="A142">
-            <v>41505</v>
-          </cell>
-        </row>
-        <row r="143">
-          <cell r="A143">
-            <v>41505</v>
-          </cell>
-        </row>
-        <row r="144">
-          <cell r="A144">
-            <v>41505</v>
-          </cell>
-        </row>
-        <row r="145">
-          <cell r="A145">
-            <v>41505</v>
-          </cell>
-        </row>
-        <row r="146">
-          <cell r="A146">
-            <v>41505</v>
-          </cell>
-        </row>
-        <row r="147">
-          <cell r="A147">
-            <v>41505</v>
-          </cell>
-        </row>
-        <row r="148">
-          <cell r="A148">
-            <v>41505</v>
-          </cell>
-        </row>
-        <row r="149">
-          <cell r="A149">
-            <v>41506</v>
-          </cell>
-        </row>
-        <row r="150">
-          <cell r="A150">
-            <v>41506</v>
-          </cell>
-        </row>
-        <row r="151">
-          <cell r="A151">
-            <v>41506</v>
-          </cell>
-        </row>
-        <row r="152">
-          <cell r="A152">
-            <v>41506</v>
-          </cell>
-        </row>
-        <row r="153">
-          <cell r="A153">
-            <v>41506</v>
-          </cell>
-        </row>
-        <row r="154">
-          <cell r="A154">
-            <v>41506</v>
-          </cell>
-        </row>
-        <row r="155">
-          <cell r="A155">
-            <v>41506</v>
-          </cell>
-        </row>
-        <row r="156">
-          <cell r="A156">
-            <v>41506</v>
-          </cell>
-        </row>
-        <row r="157">
-          <cell r="A157">
-            <v>41506</v>
-          </cell>
-        </row>
-        <row r="158">
-          <cell r="A158">
-            <v>41506</v>
-          </cell>
-        </row>
-        <row r="159">
-          <cell r="A159">
-            <v>41506</v>
-          </cell>
-        </row>
-        <row r="160">
-          <cell r="A160">
-            <v>41506</v>
-          </cell>
-        </row>
-        <row r="161">
-          <cell r="A161">
-            <v>41506</v>
-          </cell>
-        </row>
-        <row r="162">
-          <cell r="A162">
-            <v>41507</v>
-          </cell>
-        </row>
-        <row r="163">
-          <cell r="A163">
-            <v>41507</v>
-          </cell>
-        </row>
-        <row r="164">
-          <cell r="A164">
-            <v>41507</v>
-          </cell>
-        </row>
-        <row r="165">
-          <cell r="A165">
-            <v>41507</v>
-          </cell>
-        </row>
-        <row r="166">
-          <cell r="A166">
-            <v>41507</v>
-          </cell>
-        </row>
-        <row r="167">
-          <cell r="A167">
-            <v>41508</v>
-          </cell>
-        </row>
-        <row r="168">
-          <cell r="A168">
-            <v>41508</v>
-          </cell>
-        </row>
-        <row r="169">
-          <cell r="A169">
-            <v>41508</v>
-          </cell>
-        </row>
-        <row r="170">
-          <cell r="A170">
-            <v>41508</v>
-          </cell>
-        </row>
-        <row r="171">
-          <cell r="A171">
-            <v>41509</v>
-          </cell>
-        </row>
-        <row r="172">
-          <cell r="A172">
-            <v>41509</v>
-          </cell>
-        </row>
-        <row r="173">
-          <cell r="A173">
-            <v>41509</v>
-          </cell>
-        </row>
-        <row r="174">
-          <cell r="A174">
-            <v>41510</v>
-          </cell>
-        </row>
-        <row r="175">
-          <cell r="A175">
-            <v>41510</v>
-          </cell>
-        </row>
-        <row r="176">
-          <cell r="A176">
-            <v>41510</v>
-          </cell>
-        </row>
-        <row r="177">
-          <cell r="A177">
-            <v>41510</v>
-          </cell>
-        </row>
-        <row r="178">
-          <cell r="A178">
-            <v>41510</v>
-          </cell>
-        </row>
-        <row r="179">
-          <cell r="A179">
-            <v>41510</v>
-          </cell>
-        </row>
-        <row r="180">
-          <cell r="A180">
-            <v>41511</v>
-          </cell>
-        </row>
-        <row r="181">
-          <cell r="A181">
-            <v>41511</v>
-          </cell>
-        </row>
-        <row r="182">
-          <cell r="A182">
-            <v>41511</v>
-          </cell>
-        </row>
-        <row r="183">
-          <cell r="A183">
-            <v>41511</v>
-          </cell>
-        </row>
-        <row r="184">
-          <cell r="A184">
-            <v>41511</v>
-          </cell>
-        </row>
-        <row r="185">
-          <cell r="A185">
-            <v>41511</v>
-          </cell>
-        </row>
-        <row r="186">
-          <cell r="A186">
-            <v>41511</v>
-          </cell>
-        </row>
-        <row r="187">
-          <cell r="A187">
-            <v>41511</v>
-          </cell>
-        </row>
-        <row r="188">
-          <cell r="A188">
-            <v>41512</v>
-          </cell>
-        </row>
-        <row r="189">
-          <cell r="A189">
-            <v>41512</v>
-          </cell>
-        </row>
-        <row r="190">
-          <cell r="A190">
-            <v>41512</v>
-          </cell>
-        </row>
-        <row r="191">
-          <cell r="A191">
-            <v>41512</v>
-          </cell>
-        </row>
-        <row r="192">
-          <cell r="A192">
-            <v>41512</v>
-          </cell>
-        </row>
-        <row r="193">
-          <cell r="A193">
-            <v>41512</v>
-          </cell>
-        </row>
-        <row r="194">
-          <cell r="A194">
-            <v>41512</v>
-          </cell>
-        </row>
-        <row r="195">
-          <cell r="A195">
-            <v>41512</v>
-          </cell>
-        </row>
-        <row r="196">
-          <cell r="A196">
-            <v>41513</v>
-          </cell>
-        </row>
-        <row r="197">
-          <cell r="A197">
-            <v>41513</v>
-          </cell>
-        </row>
-        <row r="198">
-          <cell r="A198">
-            <v>41513</v>
-          </cell>
-        </row>
-        <row r="199">
-          <cell r="A199">
-            <v>41513</v>
-          </cell>
-        </row>
-        <row r="200">
-          <cell r="A200">
-            <v>41513</v>
-          </cell>
-        </row>
-        <row r="201">
-          <cell r="A201">
-            <v>41513</v>
-          </cell>
-        </row>
-        <row r="202">
-          <cell r="A202">
-            <v>41513</v>
-          </cell>
-        </row>
-        <row r="203">
-          <cell r="A203">
-            <v>41513</v>
-          </cell>
-        </row>
-        <row r="204">
-          <cell r="A204">
-            <v>41513</v>
-          </cell>
-        </row>
-        <row r="205">
-          <cell r="A205">
-            <v>41514</v>
-          </cell>
-        </row>
-        <row r="206">
-          <cell r="A206">
-            <v>41514</v>
-          </cell>
-        </row>
-        <row r="207">
-          <cell r="A207">
-            <v>41514</v>
-          </cell>
-        </row>
-        <row r="208">
-          <cell r="A208">
-            <v>41514</v>
-          </cell>
-        </row>
-        <row r="209">
-          <cell r="A209">
-            <v>41514</v>
-          </cell>
-        </row>
-        <row r="210">
-          <cell r="A210">
-            <v>41514</v>
-          </cell>
-        </row>
-        <row r="211">
-          <cell r="A211">
-            <v>41514</v>
-          </cell>
-        </row>
-        <row r="212">
-          <cell r="A212">
-            <v>41514</v>
-          </cell>
-        </row>
-        <row r="213">
-          <cell r="A213">
-            <v>41514</v>
-          </cell>
-        </row>
-        <row r="214">
-          <cell r="A214">
-            <v>41514</v>
-          </cell>
-        </row>
-        <row r="216">
-          <cell r="A216">
-            <v>41515</v>
-          </cell>
-        </row>
-        <row r="217">
-          <cell r="A217">
-            <v>41515</v>
-          </cell>
-        </row>
-        <row r="218">
-          <cell r="A218">
-            <v>41515</v>
-          </cell>
-        </row>
-        <row r="219">
-          <cell r="A219">
-            <v>41515</v>
-          </cell>
-        </row>
-        <row r="220">
-          <cell r="A220">
-            <v>41515</v>
-          </cell>
-        </row>
-        <row r="221">
-          <cell r="A221">
-            <v>41515</v>
-          </cell>
-        </row>
-        <row r="222">
-          <cell r="A222">
-            <v>41516</v>
-          </cell>
-        </row>
-        <row r="223">
-          <cell r="A223">
-            <v>41516</v>
-          </cell>
-        </row>
-        <row r="224">
-          <cell r="A224">
-            <v>41516</v>
-          </cell>
-        </row>
-        <row r="225">
-          <cell r="A225">
-            <v>41516</v>
-          </cell>
-        </row>
-        <row r="226">
-          <cell r="A226">
-            <v>41517</v>
-          </cell>
-        </row>
-        <row r="227">
-          <cell r="A227">
-            <v>41517</v>
-          </cell>
-        </row>
-        <row r="228">
-          <cell r="A228">
-            <v>41517</v>
-          </cell>
-        </row>
-        <row r="229">
-          <cell r="A229">
-            <v>41517</v>
-          </cell>
-        </row>
-        <row r="230">
-          <cell r="A230">
-            <v>41517</v>
-          </cell>
-          <cell r="J230">
-            <v>0.97</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="8">
-        <row r="2">
-          <cell r="A2">
-            <v>41518</v>
-          </cell>
-        </row>
-        <row r="207">
-          <cell r="A207">
-            <v>41547</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="9">
-        <row r="2">
-          <cell r="A2">
-            <v>41548</v>
-          </cell>
-        </row>
-        <row r="235">
-          <cell r="A235">
-            <v>41578</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6464,8 +5202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6510,35 +5248,27 @@
         <v>17</v>
       </c>
       <c r="B3" s="3">
-        <f>COUNT([1]March!$A$2:'[1]March'!$A$795)</f>
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C3" s="1">
-        <f>COUNT([1]April!$A$2:'[1]April'!$A$462)</f>
         <v>461</v>
       </c>
       <c r="D3" s="1">
-        <f>COUNT([1]May!$A$2:'[1]May'!$A$285)</f>
         <v>284</v>
       </c>
       <c r="E3" s="1">
-        <f>COUNT([1]June!$A$2:'[1]June'!$A$229)</f>
         <v>228</v>
       </c>
       <c r="F3" s="1">
-        <f>COUNT([1]July!$A$2:'[1]July'!$A$239)</f>
         <v>238</v>
       </c>
       <c r="G3" s="1">
-        <f>COUNT([1]August!$A$2:'[1]August'!$A$230)</f>
         <v>229</v>
       </c>
       <c r="H3" s="1">
-        <f>COUNT([1]September!$A$2:'[1]September'!$A$207)</f>
         <v>206</v>
       </c>
       <c r="I3" s="5">
-        <f>COUNT([1]October!$A$2:'[1]October'!$A$235)</f>
         <v>234</v>
       </c>
     </row>
@@ -6547,31 +5277,24 @@
         <v>18</v>
       </c>
       <c r="B4" s="3">
-        <f>COUNT([1]April!$A$2:'[1]April'!$A$462)</f>
         <v>461</v>
       </c>
       <c r="C4" s="1">
-        <f>COUNT([1]May!$A$2:'[1]May'!$A$285)</f>
         <v>284</v>
       </c>
       <c r="D4" s="1">
-        <f>COUNT([1]June!$A$2:'[1]June'!$A$229)</f>
         <v>228</v>
       </c>
       <c r="E4" s="1">
-        <f>COUNT([1]July!$A$2:'[1]July'!$A$239)</f>
         <v>238</v>
       </c>
       <c r="F4" s="1">
-        <f>COUNT([1]August!$A$2:'[1]August'!$A$230)</f>
         <v>229</v>
       </c>
       <c r="G4" s="1">
-        <f>COUNT([1]September!$A$2:'[1]September'!$A$207)</f>
         <v>206</v>
       </c>
-      <c r="H4" s="1">
-        <f>COUNT([1]October!$A$2:'[1]October'!$A$235)</f>
+      <c r="H4" s="5">
         <v>234</v>
       </c>
     </row>
@@ -6580,28 +5303,22 @@
         <v>19</v>
       </c>
       <c r="B5" s="7">
-        <f>SUM([1]March!$J$2:'[1]March'!$J$795)</f>
-        <v>804.47000999999511</v>
+        <v>804.47</v>
       </c>
       <c r="C5" s="2">
-        <f>SUM([1]April!$J$2:'[1]April'!$J$462)</f>
-        <v>426.87908600000213</v>
+        <v>426.87</v>
       </c>
       <c r="D5" s="2">
-        <f>SUM([1]May!$J$2:'[1]May'!$J$285)</f>
-        <v>253.22090599999942</v>
+        <v>253.22</v>
       </c>
       <c r="E5" s="2">
-        <f>SUM([1]June!$J$2:'[1]June'!$J$229)</f>
-        <v>212.50666799999968</v>
+        <v>212.5</v>
       </c>
       <c r="F5" s="2">
-        <f>SUM([1]July!$J$2:'[1]July'!$J$239)</f>
-        <v>202.74083299999978</v>
+        <v>202.74</v>
       </c>
       <c r="G5" s="8">
-        <f>SUM([1]August!$J$2:'[1]August'!$J$230)</f>
-        <v>209.99964299999974</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -6609,24 +5326,19 @@
         <v>20</v>
       </c>
       <c r="B6" s="7">
-        <f>SUM([1]April!$J$2:'[1]April'!$J$462)</f>
-        <v>426.87908600000213</v>
+        <v>426.87</v>
       </c>
       <c r="C6" s="2">
-        <f>SUM([1]May!$J$2:'[1]May'!$J$285)</f>
-        <v>253.22090599999942</v>
+        <v>253.22</v>
       </c>
       <c r="D6" s="2">
-        <f>SUM([1]June!$J$2:'[1]June'!$J$229)</f>
-        <v>212.50666799999968</v>
+        <v>212.5</v>
       </c>
       <c r="E6" s="2">
-        <f>SUM([1]July!$J$2:'[1]July'!$J$239)</f>
-        <v>202.74083299999978</v>
-      </c>
-      <c r="F6" s="2">
-        <f>SUM([1]August!$J$2:'[1]August'!$J$230)</f>
-        <v>209.99964299999974</v>
+        <v>202.74</v>
+      </c>
+      <c r="F6" s="9">
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -6648,7 +5360,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>0.2146*G5+160.86</f>
-        <v>205.92592338779997</v>
+        <v>205.92600000000002</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -6677,8 +5389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C245"/>
+    <sheetView topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="H240" sqref="H240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8389,8 +7101,8 @@
         <v>7</v>
       </c>
       <c r="C155">
-        <f>COUNT([1]August!$A$9:$A$13)</f>
-        <v>5</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -8398,12 +7110,12 @@
         <v>155</v>
       </c>
       <c r="B156">
-        <f>COUNT([1]August!$A$9:$A$13)</f>
-        <v>5</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C156">
-        <f>COUNT([1]August!$A$14:$A$23)</f>
-        <v>10</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -8411,12 +7123,12 @@
         <v>156</v>
       </c>
       <c r="B157">
-        <f>COUNT([1]August!$A$14:$A$23)</f>
-        <v>10</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C157">
-        <f>COUNT([1]August!$A$24:$A$31)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -8424,12 +7136,12 @@
         <v>157</v>
       </c>
       <c r="B158">
-        <f>COUNT([1]August!$A$24:$A$31)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C158">
-        <f>COUNT([1]August!$A$32:$A$35)</f>
-        <v>4</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -8437,12 +7149,12 @@
         <v>158</v>
       </c>
       <c r="B159">
-        <f>COUNT([1]August!$A$32:$A$35)</f>
-        <v>4</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C159">
-        <f>COUNT([1]August!$A$36:$A$45)</f>
-        <v>10</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -8450,12 +7162,12 @@
         <v>159</v>
       </c>
       <c r="B160">
-        <f>COUNT([1]August!$A$36:$A$45)</f>
-        <v>10</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C160">
-        <f>COUNT([1]August!$A$46:$A$53)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -8463,12 +7175,12 @@
         <v>160</v>
       </c>
       <c r="B161">
-        <f>COUNT([1]August!$A$46:$A$53)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C161">
-        <f>COUNT([1]August!$A$54:$A$62)</f>
-        <v>9</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -8476,12 +7188,12 @@
         <v>161</v>
       </c>
       <c r="B162">
-        <f>COUNT([1]August!$A$54:$A$62)</f>
-        <v>9</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C162">
-        <f>COUNT([1]August!$A$63:$A$69)</f>
-        <v>7</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -8489,12 +7201,12 @@
         <v>162</v>
       </c>
       <c r="B163">
-        <f>COUNT([1]August!$A$63:$A$69)</f>
-        <v>7</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C163">
-        <f>COUNT([1]August!$A$70:$A$76)</f>
-        <v>7</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -8502,12 +7214,12 @@
         <v>163</v>
       </c>
       <c r="B164">
-        <f>COUNT([1]August!$A$70:$A$76)</f>
-        <v>7</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C164">
-        <f>COUNT([1]August!$A$77:$A$84)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -8515,12 +7227,12 @@
         <v>164</v>
       </c>
       <c r="B165">
-        <f>COUNT([1]August!$A$77:$A$84)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C165">
-        <f>COUNT([1]August!$A$85:$A$91)</f>
-        <v>7</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -8528,12 +7240,12 @@
         <v>165</v>
       </c>
       <c r="B166">
-        <f>COUNT([1]August!$A$85:$A$91)</f>
-        <v>7</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C166">
-        <f>COUNT([1]August!$A$92:$A$105)</f>
-        <v>14</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -8541,12 +7253,12 @@
         <v>166</v>
       </c>
       <c r="B167">
-        <f>COUNT([1]August!$A$92:$A$105)</f>
-        <v>14</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C167">
-        <f>COUNT([1]August!$A$106:$A$111)</f>
-        <v>6</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -8554,12 +7266,12 @@
         <v>167</v>
       </c>
       <c r="B168">
-        <f>COUNT([1]August!$A$106:$A$111)</f>
-        <v>6</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C168">
-        <f>COUNT([1]August!$A$112:$A$117)</f>
-        <v>6</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -8567,12 +7279,12 @@
         <v>168</v>
       </c>
       <c r="B169">
-        <f>COUNT([1]August!$A$112:$A$117)</f>
-        <v>6</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C169">
-        <f>COUNT([1]August!$A$118:$A$124)</f>
-        <v>7</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -8580,12 +7292,12 @@
         <v>169</v>
       </c>
       <c r="B170">
-        <f>COUNT([1]August!$A$118:$A$124)</f>
-        <v>7</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C170">
-        <f>COUNT([1]August!$A$125:$A$131)</f>
-        <v>7</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -8593,12 +7305,12 @@
         <v>170</v>
       </c>
       <c r="B171">
-        <f>COUNT([1]August!$A$125:$A$131)</f>
-        <v>7</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C171">
-        <f>COUNT([1]August!$A$132:$A$140)</f>
-        <v>9</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -8606,12 +7318,12 @@
         <v>171</v>
       </c>
       <c r="B172">
-        <f>COUNT([1]August!$A$132:$A$140)</f>
-        <v>9</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C172">
-        <f>COUNT([1]August!$A$141:$A$148)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -8619,12 +7331,12 @@
         <v>172</v>
       </c>
       <c r="B173">
-        <f>COUNT([1]August!$A$141:$A$148)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C173">
-        <f>COUNT([1]August!$A$149:$A$161)</f>
-        <v>13</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -8632,12 +7344,12 @@
         <v>173</v>
       </c>
       <c r="B174">
-        <f>COUNT([1]August!$A$149:$A$161)</f>
-        <v>13</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C174">
-        <f>COUNT([1]August!$A$162:$A$166)</f>
-        <v>5</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -8645,12 +7357,12 @@
         <v>174</v>
       </c>
       <c r="B175">
-        <f>COUNT([1]August!$A$162:$A$166)</f>
-        <v>5</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C175">
-        <f>COUNT([1]August!$A$167:$A$170)</f>
-        <v>4</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -8658,12 +7370,12 @@
         <v>175</v>
       </c>
       <c r="B176">
-        <f>COUNT([1]August!$A$167:$A$170)</f>
-        <v>4</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C176">
-        <f>COUNT([1]August!$A$171:$A$173)</f>
-        <v>3</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -8671,12 +7383,12 @@
         <v>176</v>
       </c>
       <c r="B177">
-        <f>COUNT([1]August!$A$171:$A$173)</f>
-        <v>3</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C177">
-        <f>COUNT([1]August!$A$174:$A$179)</f>
-        <v>6</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -8684,12 +7396,12 @@
         <v>177</v>
       </c>
       <c r="B178">
-        <f>COUNT([1]August!$A$174:$A$179)</f>
-        <v>6</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C178">
-        <f>COUNT([1]August!$A$180:$A$187)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -8697,12 +7409,12 @@
         <v>178</v>
       </c>
       <c r="B179">
-        <f>COUNT([1]August!$A$180:$A$187)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C179">
-        <f>COUNT([1]August!$A$188:$A$195)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -8710,12 +7422,12 @@
         <v>179</v>
       </c>
       <c r="B180">
-        <f>COUNT([1]August!$A$188:$A$195)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C180">
-        <f>COUNT([1]August!$A$196:$A$204)</f>
-        <v>9</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -8723,12 +7435,12 @@
         <v>180</v>
       </c>
       <c r="B181">
-        <f>COUNT([1]August!$A$196:$A$204)</f>
-        <v>9</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C181">
-        <f>COUNT([1]August!$A$205:$A$214)</f>
-        <v>10</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -8736,12 +7448,12 @@
         <v>181</v>
       </c>
       <c r="B182">
-        <f>COUNT([1]August!$A$205:$A$214)</f>
-        <v>10</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C182">
-        <f>COUNT([1]August!$A$216:$A$221)</f>
-        <v>6</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -8749,12 +7461,12 @@
         <v>182</v>
       </c>
       <c r="B183">
-        <f>COUNT([1]August!$A$216:$A$221)</f>
-        <v>6</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C183">
-        <f>COUNT([1]August!$A$222:$A$225)</f>
-        <v>4</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -8762,12 +7474,12 @@
         <v>183</v>
       </c>
       <c r="B184">
-        <f>COUNT([1]August!$A$222:$A$225)</f>
-        <v>4</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C184">
-        <f>COUNT([1]August!$A$226:$A$230)</f>
-        <v>5</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -8775,8 +7487,8 @@
         <v>184</v>
       </c>
       <c r="B185">
-        <f>COUNT([1]August!$A$226:$A$230)</f>
-        <v>5</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
       <c r="C185">
         <v>5</v>
@@ -9464,7 +8176,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:H33"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10930,8 +9642,8 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <f>COUNT([1]August!$A$9:$A$13)</f>
-        <v>5</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -10939,8 +9651,8 @@
         <v>3</v>
       </c>
       <c r="G4">
-        <f>COUNT([1]August!$A$14:$A$23)</f>
-        <v>10</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -10948,8 +9660,8 @@
         <v>4</v>
       </c>
       <c r="H5">
-        <f>COUNT([1]August!$A$24:$A$31)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -10957,8 +9669,8 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <f>COUNT([1]August!$A$32:$A$35)</f>
-        <v>4</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -10966,8 +9678,8 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <f>COUNT([1]August!$A$36:$A$45)</f>
-        <v>10</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -10975,8 +9687,8 @@
         <v>7</v>
       </c>
       <c r="D8">
-        <f>COUNT([1]August!$A$46:$A$53)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -10984,8 +9696,8 @@
         <v>8</v>
       </c>
       <c r="E9">
-        <f>COUNT([1]August!$A$54:$A$62)</f>
-        <v>9</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -10993,8 +9705,8 @@
         <v>9</v>
       </c>
       <c r="F10">
-        <f>COUNT([1]August!$A$63:$A$69)</f>
-        <v>7</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -11002,8 +9714,8 @@
         <v>10</v>
       </c>
       <c r="G11">
-        <f>COUNT([1]August!$A$70:$A$76)</f>
-        <v>7</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -11011,8 +9723,8 @@
         <v>11</v>
       </c>
       <c r="H12">
-        <f>COUNT([1]August!$A$77:$A$84)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -11020,8 +9732,8 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <f>COUNT([1]August!$A$85:$A$91)</f>
-        <v>7</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -11029,8 +9741,8 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <f>COUNT([1]August!$A$92:$A$105)</f>
-        <v>14</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -11038,8 +9750,8 @@
         <v>14</v>
       </c>
       <c r="D15">
-        <f>COUNT([1]August!$A$106:$A$111)</f>
-        <v>6</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -11047,8 +9759,8 @@
         <v>15</v>
       </c>
       <c r="E16">
-        <f>COUNT([1]August!$A$112:$A$117)</f>
-        <v>6</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -11056,8 +9768,8 @@
         <v>16</v>
       </c>
       <c r="F17">
-        <f>COUNT([1]August!$A$118:$A$124)</f>
-        <v>7</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -11065,8 +9777,8 @@
         <v>17</v>
       </c>
       <c r="G18">
-        <f>COUNT([1]August!$A$125:$A$131)</f>
-        <v>7</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -11074,8 +9786,8 @@
         <v>18</v>
       </c>
       <c r="H19">
-        <f>COUNT([1]August!$A$132:$A$140)</f>
-        <v>9</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -11083,8 +9795,8 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <f>COUNT([1]August!$A$141:$A$148)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -11092,8 +9804,8 @@
         <v>20</v>
       </c>
       <c r="C21">
-        <f>COUNT([1]August!$A$149:$A$161)</f>
-        <v>13</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -11101,8 +9813,8 @@
         <v>21</v>
       </c>
       <c r="D22">
-        <f>COUNT([1]August!$A$162:$A$166)</f>
-        <v>5</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -11110,8 +9822,8 @@
         <v>22</v>
       </c>
       <c r="E23">
-        <f>COUNT([1]August!$A$167:$A$170)</f>
-        <v>4</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -11119,8 +9831,8 @@
         <v>23</v>
       </c>
       <c r="F24">
-        <f>COUNT([1]August!$A$171:$A$173)</f>
-        <v>3</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -11128,8 +9840,8 @@
         <v>24</v>
       </c>
       <c r="G25">
-        <f>COUNT([1]August!$A$174:$A$179)</f>
-        <v>6</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -11137,8 +9849,8 @@
         <v>25</v>
       </c>
       <c r="H26">
-        <f>COUNT([1]August!$A$180:$A$187)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -11146,8 +9858,8 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <f>COUNT([1]August!$A$188:$A$195)</f>
-        <v>8</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -11155,8 +9867,8 @@
         <v>27</v>
       </c>
       <c r="C28">
-        <f>COUNT([1]August!$A$196:$A$204)</f>
-        <v>9</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -11164,8 +9876,8 @@
         <v>28</v>
       </c>
       <c r="D29">
-        <f>COUNT([1]August!$A$205:$A$214)</f>
-        <v>10</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -11173,8 +9885,8 @@
         <v>29</v>
       </c>
       <c r="E30">
-        <f>COUNT([1]August!$A$216:$A$221)</f>
-        <v>6</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -11182,8 +9894,8 @@
         <v>30</v>
       </c>
       <c r="F31">
-        <f>COUNT([1]August!$A$222:$A$225)</f>
-        <v>4</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -11191,8 +9903,8 @@
         <v>31</v>
       </c>
       <c r="G32">
-        <f>COUNT([1]August!$A$226:$A$230)</f>
-        <v>5</v>
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Put outline in report. Provided outline in pdf format, and put r^2 formula on one of the prediction charts.
</commit_message>
<xml_diff>
--- a/App Data - Prediction.xlsx
+++ b/App Data - Prediction.xlsx
@@ -23,9 +23,6 @@
     <sheet name="Day of Week Pred Oct" sheetId="9" r:id="rId9"/>
     <sheet name="Prediction" sheetId="10" r:id="rId10"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId11"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -332,7 +329,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
@@ -435,11 +432,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1333934224"/>
-        <c:axId val="1333932048"/>
+        <c:axId val="-1844292032"/>
+        <c:axId val="-1844285504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1333934224"/>
+        <c:axId val="-1844292032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,12 +554,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1333932048"/>
+        <c:crossAx val="-1844285504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1333932048"/>
+        <c:axId val="-1844285504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -680,7 +677,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1333934224"/>
+        <c:crossAx val="-1844292032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -931,11 +928,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1333934768"/>
-        <c:axId val="1333933136"/>
+        <c:axId val="-1844294752"/>
+        <c:axId val="-1844280608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1333934768"/>
+        <c:axId val="-1844294752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1052,12 +1049,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1333933136"/>
+        <c:crossAx val="-1844280608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1333933136"/>
+        <c:axId val="-1844280608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1175,7 +1172,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1333934768"/>
+        <c:crossAx val="-1844294752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1269,7 +1266,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1344,7 +1340,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2867,11 +2862,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1333938576"/>
-        <c:axId val="1333939120"/>
+        <c:axId val="-1844283328"/>
+        <c:axId val="-1844286048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1333938576"/>
+        <c:axId val="-1844283328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2917,7 +2912,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2984,12 +2978,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1333939120"/>
+        <c:crossAx val="-1844286048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1333939120"/>
+        <c:axId val="-1844286048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3040,7 +3034,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3107,7 +3100,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1333938576"/>
+        <c:crossAx val="-1844283328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4924,19 +4917,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5203,7 +5183,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>